<commit_message>
Did some Excel stuff
Updated Excel sheet of current consumptions with more real values.
Added "real" NRF24L01 times.
Plan is to power off NRF24L01 in SLEEP period.
</commit_message>
<xml_diff>
--- a/NRF24L01 current consumption.xlsx
+++ b/NRF24L01 current consumption.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
     <sheet name="NRF24L01" sheetId="2" r:id="rId2"/>
+    <sheet name="Capacitor" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>min</t>
   </si>
@@ -153,10 +154,37 @@
     <t>NRF24L01 TX -18dBm @ 2Mbits</t>
   </si>
   <si>
-    <t>RTC</t>
-  </si>
-  <si>
     <t>74AUP373</t>
+  </si>
+  <si>
+    <t>TLP5010</t>
+  </si>
+  <si>
+    <t>Etc.</t>
+  </si>
+  <si>
+    <t>Peak current</t>
+  </si>
+  <si>
+    <t>Time at peak</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>mV</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>mW</t>
+  </si>
+  <si>
+    <t>uW</t>
   </si>
 </sst>
 </file>
@@ -230,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -246,12 +274,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,9 +284,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -311,6 +330,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,6 +427,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -410,6 +447,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -425,6 +467,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -440,6 +487,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="4"/>
@@ -455,6 +507,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="5"/>
@@ -470,6 +527,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000B-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="6"/>
@@ -487,6 +549,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000D-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="7"/>
@@ -504,6 +571,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="8"/>
@@ -521,6 +593,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000011-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="9"/>
@@ -538,6 +615,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="10"/>
@@ -555,6 +637,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="11"/>
@@ -572,6 +659,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="12"/>
@@ -590,6 +682,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="13"/>
@@ -608,6 +705,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="14"/>
@@ -626,6 +728,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001D-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="15"/>
@@ -644,6 +751,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="16"/>
@@ -662,6 +774,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000021-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="17"/>
@@ -680,6 +797,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000023-5861-454B-912A-B6F6905495CC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -702,7 +824,7 @@
                   <c:v>NRF24L01 TX -18dBm @ 2Mbits</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>RTC</c:v>
+                  <c:v>TLP5010</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>NRF standby</c:v>
@@ -753,7 +875,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3050913900388778E-2</c:v>
+                  <c:v>0.22802220759432015</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -765,7 +887,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9385107452088501</c:v>
+                  <c:v>1.2268515654916423</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -774,19 +896,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2115692157555313E-2</c:v>
+                  <c:v>4.381612733898723E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>94.642803504600721</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>96.92550495193008</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.6154256210073752E-4</c:v>
+                  <c:v>5.8421503118649644E-4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2.2083328178849563E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -795,10 +917,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.9691584470671647</c:v>
+                  <c:v>3.5049396581002665</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.1497707173857745E-2</c:v>
+                  <c:v>0.33089939366403159</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0</c:v>
@@ -1760,7 +1882,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,7 +1897,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1784,27 +1906,27 @@
       <c r="C1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="26">
+      <c r="A2" s="23">
         <v>5</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="11">
         <f>A2*60</f>
         <v>300</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="11">
         <f>B2*1000</f>
         <v>300000</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="13">
         <f>C2*1000</f>
         <v>300000000</v>
       </c>
-      <c r="E2" s="26"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1819,7 +1941,7 @@
       <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="29" t="s">
+      <c r="E4" s="26" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -1834,7 +1956,7 @@
       <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1845,11 +1967,11 @@
       <c r="B5" s="5">
         <v>11.3</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <f>B5*1000</f>
         <v>11300</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="11">
         <f>NRF24L01!G4</f>
         <v>1324.2026000000001</v>
       </c>
@@ -1872,8 +1994,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J5" s="12">
-        <f>I5/$I$23*100</f>
+      <c r="J5" s="10">
+        <f t="shared" ref="J5:J23" si="1">I5/$I$26*100</f>
         <v>0</v>
       </c>
     </row>
@@ -1884,16 +2006,16 @@
       <c r="B6" s="5">
         <v>11.3</v>
       </c>
-      <c r="C6" s="14">
-        <f t="shared" ref="C6:C14" si="1">B6*1000</f>
+      <c r="C6" s="11">
+        <f t="shared" ref="C6:C14" si="2">B6*1000</f>
         <v>11300</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="11">
         <f>NRF24L01!$G$6</f>
         <v>172.7014485</v>
       </c>
       <c r="E6" s="6">
-        <f t="shared" ref="E6:E22" si="2">D6*0.001</f>
+        <f t="shared" ref="E6:E23" si="3">D6*0.001</f>
         <v>0.17270144849999999</v>
       </c>
       <c r="F6" s="3">
@@ -1911,9 +2033,9 @@
         <f t="shared" si="0"/>
         <v>6.5050878934999998</v>
       </c>
-      <c r="J6" s="12">
-        <f>I6/$I$23*100</f>
-        <v>6.3050913900388778E-2</v>
+      <c r="J6" s="10">
+        <f t="shared" si="1"/>
+        <v>0.22802220759432015</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1923,16 +2045,16 @@
       <c r="B7" s="5">
         <v>9</v>
       </c>
-      <c r="C7" s="14">
-        <f t="shared" si="1"/>
+      <c r="C7" s="11">
+        <f t="shared" si="2"/>
         <v>9000</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="11">
         <f>NRF24L01!$G$6</f>
         <v>172.7014485</v>
       </c>
       <c r="E7" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17270144849999999</v>
       </c>
       <c r="F7" s="3">
@@ -1950,8 +2072,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J7" s="12">
-        <f>I7/$I$23*100</f>
+      <c r="J7" s="10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1962,16 +2084,16 @@
       <c r="B8" s="5">
         <v>7.5</v>
       </c>
-      <c r="C8" s="14">
-        <f t="shared" si="1"/>
+      <c r="C8" s="11">
+        <f t="shared" si="2"/>
         <v>7500</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="11">
         <f>NRF24L01!$G$6</f>
         <v>172.7014485</v>
       </c>
       <c r="E8" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17270144849999999</v>
       </c>
       <c r="F8" s="3">
@@ -1989,8 +2111,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J8" s="12">
-        <f>I8/$I$23*100</f>
+      <c r="J8" s="10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2001,16 +2123,16 @@
       <c r="B9" s="5">
         <v>7</v>
       </c>
-      <c r="C9" s="14">
-        <f t="shared" si="1"/>
+      <c r="C9" s="11">
+        <f t="shared" si="2"/>
         <v>7000</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <f>NRF24L01!$G$6</f>
         <v>172.7014485</v>
       </c>
       <c r="E9" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17270144849999999</v>
       </c>
       <c r="F9" s="3">
@@ -2028,29 +2150,29 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J9" s="12">
-        <f>I9/$I$23*100</f>
+      <c r="J9" s="10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B10" s="5">
-        <f>200*0.000001</f>
-        <v>1.9999999999999998E-4</v>
-      </c>
-      <c r="C10" s="14">
-        <f t="shared" si="1"/>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="D10" s="14">
+        <f>35*0.000001</f>
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="C10" s="11">
+        <f t="shared" si="2"/>
+        <v>3.4999999999999996E-2</v>
+      </c>
+      <c r="D10" s="11">
         <f>D2</f>
         <v>300000000</v>
       </c>
       <c r="E10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>300000</v>
       </c>
       <c r="F10" s="3">
@@ -2058,19 +2180,19 @@
       </c>
       <c r="G10" s="5">
         <f>(B10*(D10/D2))*F10</f>
-        <v>1.9999999999999998E-4</v>
+        <v>3.4999999999999997E-5</v>
       </c>
       <c r="H10" s="6">
-        <f t="shared" ref="H10:I22" si="3">G10*1000</f>
-        <v>0.19999999999999998</v>
+        <f t="shared" ref="H10:I23" si="4">G10*1000</f>
+        <v>3.4999999999999996E-2</v>
       </c>
       <c r="I10" s="6">
-        <f t="shared" si="3"/>
-        <v>199.99999999999997</v>
-      </c>
-      <c r="J10" s="12">
-        <f>I10/$I$23*100</f>
-        <v>1.9385107452088501</v>
+        <f t="shared" si="4"/>
+        <v>34.999999999999993</v>
+      </c>
+      <c r="J10" s="10">
+        <f t="shared" si="1"/>
+        <v>1.2268515654916423</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2081,16 +2203,16 @@
         <f>26*0.001</f>
         <v>2.6000000000000002E-2</v>
       </c>
-      <c r="C11" s="14">
-        <f t="shared" si="1"/>
+      <c r="C11" s="11">
+        <f t="shared" si="2"/>
         <v>26.000000000000004</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="11">
         <f>(D2-D5)</f>
         <v>299998675.7974</v>
       </c>
       <c r="E11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>299998.67579740001</v>
       </c>
       <c r="F11" s="3">
@@ -2101,15 +2223,15 @@
         <v>0</v>
       </c>
       <c r="H11" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I11" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="12">
-        <f>I11/$I$23*100</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2121,16 +2243,16 @@
         <f>900*0.000001</f>
         <v>8.9999999999999998E-4</v>
       </c>
-      <c r="C12" s="14">
-        <f t="shared" si="1"/>
+      <c r="C12" s="11">
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="11">
         <f>D2-D5</f>
         <v>299998675.7974</v>
       </c>
       <c r="E12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>299998.67579740001</v>
       </c>
       <c r="F12" s="3">
@@ -2141,15 +2263,15 @@
         <v>0</v>
       </c>
       <c r="H12" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I12" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="12">
-        <f>I12/$I$23*100</f>
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -2160,15 +2282,15 @@
       <c r="B13" s="5">
         <v>3.75</v>
       </c>
-      <c r="C13" s="14">
-        <f t="shared" si="1"/>
+      <c r="C13" s="11">
+        <f t="shared" si="2"/>
         <v>3750</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="11">
         <v>100</v>
       </c>
       <c r="E13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
       <c r="F13" s="3">
@@ -2179,16 +2301,16 @@
         <v>1.2500000000000001E-6</v>
       </c>
       <c r="H13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.25E-3</v>
       </c>
       <c r="I13" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.25</v>
       </c>
-      <c r="J13" s="12">
-        <f>I13/$I$23*100</f>
-        <v>1.2115692157555313E-2</v>
+      <c r="J13" s="10">
+        <f t="shared" si="1"/>
+        <v>4.381612733898723E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2199,36 +2321,36 @@
         <f>2.7*0.001</f>
         <v>2.7000000000000001E-3</v>
       </c>
-      <c r="C14" s="14">
-        <f t="shared" si="1"/>
+      <c r="C14" s="11">
+        <f t="shared" si="2"/>
         <v>2.7</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="11">
         <f>D2-D13</f>
         <v>299999900</v>
       </c>
       <c r="E14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>299999.90000000002</v>
       </c>
       <c r="F14" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="5">
         <f>(B14*(D14/D2))*F14</f>
-        <v>0</v>
+        <v>2.6999990999999998E-3</v>
       </c>
       <c r="H14" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.6999990999999999</v>
       </c>
       <c r="I14" s="6">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="12">
-        <f>I14/$I$23*100</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2699.9991</v>
+      </c>
+      <c r="J14" s="10">
+        <f t="shared" si="1"/>
+        <v>94.642803504600721</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2239,35 +2361,35 @@
         <f>C15*0.001</f>
         <v>0.01</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="11">
         <v>10</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="11">
         <f>D2-D13</f>
         <v>299999900</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>299999.90000000002</v>
       </c>
       <c r="F15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="5">
         <f>(B15*(D15/D2))*F15</f>
-        <v>9.9999966666666669E-3</v>
+        <v>0</v>
       </c>
       <c r="H15" s="6">
-        <f t="shared" ref="H15:I21" si="4">G15*1000</f>
-        <v>9.9999966666666662</v>
+        <f t="shared" ref="H15:I21" si="5">G15*1000</f>
+        <v>0</v>
       </c>
       <c r="I15" s="6">
-        <f t="shared" si="4"/>
-        <v>9999.996666666666</v>
-      </c>
-      <c r="J15" s="12">
-        <f>I15/$I$23*100</f>
-        <v>96.92550495193008</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2278,15 +2400,15 @@
         <f>400*0.001</f>
         <v>0.4</v>
       </c>
-      <c r="C16" s="14">
-        <f t="shared" ref="C16:C21" si="5">B16*1000</f>
+      <c r="C16" s="11">
+        <f t="shared" ref="C16:C21" si="6">B16*1000</f>
         <v>400</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="11">
         <v>12.5</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="F16" s="3">
@@ -2297,16 +2419,16 @@
         <v>1.6666666666666667E-8</v>
       </c>
       <c r="H16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6666666666666667E-5</v>
       </c>
       <c r="I16" s="6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="J16" s="12">
-        <f>I16/$I$23*100</f>
-        <v>1.6154256210073752E-4</v>
+      <c r="J16" s="10">
+        <f t="shared" si="1"/>
+        <v>5.8421503118649644E-4</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2314,255 +2436,315 @@
         <v>19</v>
       </c>
       <c r="B17" s="5">
-        <f>8*0.001</f>
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="C17" s="14">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="D17" s="14">
+        <f>C17*0.001</f>
+        <v>6.3E-7</v>
+      </c>
+      <c r="C17" s="11">
+        <v>6.3000000000000003E-4</v>
+      </c>
+      <c r="D17" s="11">
         <f>D2</f>
         <v>300000000</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>300000</v>
       </c>
       <c r="F17" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="5">
         <f>(B17*(D17/D2))*F17</f>
-        <v>0</v>
+        <v>6.3E-7</v>
       </c>
       <c r="H17" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>6.3000000000000003E-4</v>
       </c>
       <c r="I17" s="6">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="12">
-        <f>I17/$I$23*100</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.63</v>
+      </c>
+      <c r="J17" s="10">
+        <f t="shared" si="1"/>
+        <v>2.2083328178849563E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="19">
         <f>7.9*0.001</f>
         <v>7.9000000000000008E-3</v>
       </c>
-      <c r="C18" s="14">
-        <f t="shared" si="5"/>
+      <c r="C18" s="11">
+        <f t="shared" si="6"/>
         <v>7.9</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="17">
         <f>D2</f>
         <v>300000000</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>300000</v>
       </c>
-      <c r="F18" s="21">
-        <v>0</v>
-      </c>
-      <c r="G18" s="22">
-        <f>(B18*(D18/$D$2))*F18</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="23">
-        <f>I18/$I$23*100</f>
+      <c r="F18" s="18">
+        <v>0</v>
+      </c>
+      <c r="G18" s="19">
+        <f t="shared" ref="G18:G23" si="7">(B18*(D18/$D$2))*F18</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="21" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="5">
         <v>15</v>
       </c>
-      <c r="C19" s="14">
-        <f t="shared" si="5"/>
+      <c r="C19" s="11">
+        <f t="shared" si="6"/>
         <v>15000</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="11">
         <f>10*1000</f>
         <v>10000</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="F19" s="25">
-        <v>0</v>
-      </c>
-      <c r="G19" s="22">
-        <f>(B19*(D19/$D$2))*F19</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="19">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="23">
-        <f>I19/$I$23*100</f>
+      <c r="F19" s="22">
+        <v>0</v>
+      </c>
+      <c r="G19" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H19" s="16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="16">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="20">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="21" t="s">
         <v>30</v>
       </c>
       <c r="B20" s="5">
         <f>0.1*0.001</f>
         <v>1E-4</v>
       </c>
-      <c r="C20" s="14">
-        <f t="shared" si="5"/>
+      <c r="C20" s="11">
+        <f t="shared" si="6"/>
         <v>0.1</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="11">
         <f>D2-D21</f>
         <v>299970000</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>299970</v>
       </c>
-      <c r="F20" s="14">
+      <c r="F20" s="11">
         <v>1</v>
       </c>
-      <c r="G20" s="22">
-        <f>(B20*(D20/$D$2))*F20</f>
+      <c r="G20" s="19">
+        <f t="shared" si="7"/>
         <v>9.999000000000001E-5</v>
       </c>
-      <c r="H20" s="19">
-        <f t="shared" si="4"/>
+      <c r="H20" s="16">
+        <f t="shared" si="5"/>
         <v>9.9990000000000009E-2</v>
       </c>
-      <c r="I20" s="19">
-        <f t="shared" si="4"/>
+      <c r="I20" s="16">
+        <f t="shared" si="5"/>
         <v>99.990000000000009</v>
       </c>
-      <c r="J20" s="23">
-        <f>I20/$I$23*100</f>
-        <v>0.9691584470671647</v>
+      <c r="J20" s="20">
+        <f t="shared" si="1"/>
+        <v>3.5049396581002665</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="19">
         <f>94.4*0.001</f>
         <v>9.4400000000000012E-2</v>
       </c>
-      <c r="C21" s="14">
-        <f t="shared" si="5"/>
+      <c r="C21" s="11">
+        <f t="shared" si="6"/>
         <v>94.4</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="11">
         <f>30*1000</f>
         <v>30000</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="11">
         <v>1</v>
       </c>
-      <c r="G21" s="22">
-        <f>(B21*(D21/$D$2))*F21</f>
+      <c r="G21" s="19">
+        <f t="shared" si="7"/>
         <v>9.4400000000000011E-6</v>
       </c>
-      <c r="H21" s="19">
-        <f t="shared" si="4"/>
+      <c r="H21" s="16">
+        <f t="shared" si="5"/>
         <v>9.4400000000000005E-3</v>
       </c>
-      <c r="I21" s="19">
-        <f t="shared" si="4"/>
+      <c r="I21" s="16">
+        <f t="shared" si="5"/>
         <v>9.4400000000000013</v>
       </c>
-      <c r="J21" s="23">
-        <f>I21/$I$23*100</f>
-        <v>9.1497707173857745E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="7">
+      <c r="J21" s="20">
+        <f t="shared" si="1"/>
+        <v>0.33089939366403159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="19">
         <f>C22*0.001</f>
         <v>1.4E-3</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="17">
         <v>1.4</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="17">
         <f>$D$2</f>
         <v>300000000</v>
       </c>
-      <c r="E22" s="8">
-        <f t="shared" si="2"/>
+      <c r="E22" s="16">
+        <f t="shared" si="3"/>
         <v>300000</v>
       </c>
-      <c r="F22" s="15">
-        <v>0</v>
-      </c>
-      <c r="G22" s="7">
-        <f>(B22*(D22/$D$2))*F22</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="8">
+      <c r="F22" s="17">
+        <v>0</v>
+      </c>
+      <c r="G22" s="19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H22" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="5">
+        <f>C23*0.001</f>
+        <v>6.6E-4</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.66</v>
+      </c>
+      <c r="D23" s="11">
+        <f>$D$2</f>
+        <v>300000000</v>
+      </c>
+      <c r="E23" s="16">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="8">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J22" s="13">
-        <f>I22/$I$23*100</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="9">
-        <f>SUM(G5:G22)</f>
-        <v>1.0317198421226833E-2</v>
-      </c>
-      <c r="H23" s="10">
-        <f>G23*1000</f>
-        <v>10.317198421226832</v>
-      </c>
-      <c r="I23" s="10">
-        <f t="shared" ref="I23" si="6">H23*1000</f>
-        <v>10317.198421226833</v>
-      </c>
-      <c r="J23" s="12">
-        <f>SUM(J5:J22)</f>
-        <v>99.999999999999986</v>
+        <v>300000</v>
+      </c>
+      <c r="F23" s="27">
+        <v>0</v>
+      </c>
+      <c r="G23" s="28">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J23" s="30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G26" s="7">
+        <f>SUM(G5:G23)</f>
+        <v>2.8528308545601663E-3</v>
+      </c>
+      <c r="H26" s="8">
+        <f>G26*1000</f>
+        <v>2.8528308545601662</v>
+      </c>
+      <c r="I26" s="8">
+        <f t="shared" ref="I26" si="8">H26*1000</f>
+        <v>2852.8308545601662</v>
+      </c>
+      <c r="J26" s="10">
+        <f>SUM(J5:J23)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -2575,10 +2757,10 @@
       <c r="C29" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2586,76 +2768,76 @@
       <c r="A30" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="11">
         <v>210</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="11">
         <v>80</v>
       </c>
-      <c r="D30" s="17">
-        <f>(B30*0.8)/G23/24</f>
-        <v>678.47876082309756</v>
-      </c>
-      <c r="E30" s="17">
+      <c r="D30" s="14">
+        <f>((B30*0.8)/G26)/24</f>
+        <v>2453.7031309832851</v>
+      </c>
+      <c r="E30" s="14">
         <f>D30/365</f>
-        <v>1.858845920063281</v>
+        <v>6.7224743314610551</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="11">
         <v>500</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="11">
         <v>80</v>
       </c>
-      <c r="D31" s="17">
-        <f>(B31*0.8)/G23/24</f>
-        <v>1615.4256210073752</v>
-      </c>
-      <c r="E31" s="17">
+      <c r="D31" s="14">
+        <f>(B31*0.8)/G26/24</f>
+        <v>5842.1503118649634</v>
+      </c>
+      <c r="E31" s="14">
         <f>D31/365</f>
-        <v>4.4258236191982885</v>
+        <v>16.005891265383461</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="11">
         <v>560</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="11">
         <v>80</v>
       </c>
-      <c r="D32" s="17">
-        <f>(B32*0.8)/$G$23/24</f>
-        <v>1809.2766955282602</v>
-      </c>
-      <c r="E32" s="17">
+      <c r="D32" s="14">
+        <f>(B32*0.8)/$G$26/24</f>
+        <v>6543.2083492887587</v>
+      </c>
+      <c r="E32" s="14">
         <f>D32/365</f>
-        <v>4.9569224535020826</v>
+        <v>17.926598217229476</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="14">
+      <c r="B33" s="11">
         <v>2000</v>
       </c>
-      <c r="C33" s="14">
+      <c r="C33" s="11">
         <v>70</v>
       </c>
-      <c r="D33" s="17">
-        <f>(B33*C33/100)/$G$23/24</f>
-        <v>5653.9896735258126</v>
-      </c>
-      <c r="E33" s="17">
+      <c r="D33" s="14">
+        <f>(B33*C33/100)/$G$26/24</f>
+        <v>20447.526091527372</v>
+      </c>
+      <c r="E33" s="14">
         <f>D33/365</f>
-        <v>15.490382667194007</v>
+        <v>56.020619428842117</v>
       </c>
     </row>
   </sheetData>
@@ -2667,19 +2849,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
         <v>34</v>
       </c>
       <c r="B1">
@@ -2731,7 +2914,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="26">
+      <c r="A4" s="23">
         <v>0.25</v>
       </c>
       <c r="B4">
@@ -2760,7 +2943,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
+      <c r="A5" s="23">
         <v>1</v>
       </c>
       <c r="B5">
@@ -2789,7 +2972,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="26">
+      <c r="A6" s="23">
         <v>2</v>
       </c>
       <c r="B6">
@@ -2839,6 +3022,91 @@
       </c>
       <c r="B13">
         <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="31">
+        <f>'Ark1'!E6</f>
+        <v>0.17270144849999999</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>3000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23">
+        <f>(B20*0.001)*(B22*0.001)^2*(B21*0.001)</f>
+        <v>2.3314695547500002E-5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <f>B23*1000</f>
+        <v>2.33146955475E-2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <f>B23*1000000</f>
+        <v>23.314695547500001</v>
+      </c>
+      <c r="C25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>0.5*0.01*3^2</f>
+        <v>4.4999999999999998E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>